<commit_message>
update: testset; swipl c interface
</commit_message>
<xml_diff>
--- a/src/Samples/PlanSelection/PlanAssistant/scripts/TestSet.xlsx
+++ b/src/Samples/PlanSelection/PlanAssistant/scripts/TestSet.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10209"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28429"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/faisalwaris/repos/RTOpenAI/src/Samples/PlanSelection/PlanAssistant/scripts/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\s\repos\RTOpenAI\src\Samples\PlanSelection\PlanAssistant\scripts\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{37F6061A-C859-AD46-9FCA-2695A067855B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{79407D8F-DA5C-4F7C-B367-8D9064A8C6A8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="680" windowWidth="25600" windowHeight="14320" xr2:uid="{92FAE82D-58B3-3F4F-8F03-CAD8585F1368}"/>
+    <workbookView xWindow="-20600" yWindow="610" windowWidth="20550" windowHeight="16780" xr2:uid="{92FAE82D-58B3-3F4F-8F03-CAD8585F1368}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="42">
   <si>
     <t>Question</t>
   </si>
@@ -90,6 +90,137 @@
   </si>
   <si>
     <t>List the plans which offer the most highspeed hotspot data</t>
+  </si>
+  <si>
+    <t>1: Title=Connect Plus; MaxDataLimit=50
+2: Title=Connect Next First Responder; MaxDataLimit=50
+3: Title=Connect Next 55; MaxDataLimit=50
+4: Title=Connect Plus First Responder; MaxDataLimit=50
+5: Title=Connect Plus Military; MaxDataLimit=50
+6: Title=Connect Next; MaxDataLimit=50</t>
+  </si>
+  <si>
+    <t>plan_mobile_hotspot_data(Title, DataLimit) :-
+    plan(Title, _, _, features(Features)),
+    member(feature(mobile_hotspot(_, high_speed_data_limit_gb(DataLimit)), _), Features).
+most_mobile_hotspot_plan(Title, MaxDataLimit) :-
+    findall(D, plan_mobile_hotspot_data(_, D), DataList),
+    max_list(DataList, MaxDataLimit),
+    plan_mobile_hotspot_data(Title, MaxDataLimit).</t>
+  </si>
+  <si>
+    <t>most_mobile_hotspot_plan(Title, MaxDataLimit).</t>
+  </si>
+  <si>
+    <t>Are there any plans for first responders? If so what are their prices for 4 lines.</t>
+  </si>
+  <si>
+    <t>1: Title=Connect Next First Responder; Price=200
+2: Title=Connect Plus First Responder; Price=160
+3: Title=Connect First Responder; Price=120</t>
+  </si>
+  <si>
+    <t>plan_for_first_responder(Title, Price) :-
+    plan(Title, category(first_responder), lines(Lines), _),
+    member(line(4, monthly_price(Price), _), Lines).</t>
+  </si>
+  <si>
+    <t>plan_for_first_responder(Title, Price).</t>
+  </si>
+  <si>
+    <t>Find all available plans that can support 3 lines. Give their names and cost for 3 lines.</t>
+  </si>
+  <si>
+    <t>1: Title=Connect Plus; Price=150
+2: Title=Connect Next First Responder; Price=165
+3: Title=Core Saver; Price=100
+4: Title=Connect Next 55; Price=195
+5: Title=Core; Price=90
+6: Title=Connect Next Military; Price=165
+7: Title=Connect Plus 55; Price=165
+8: Title=Connect Plus First Responder; Price=135
+9: Title=Connect Plus Military; Price=135
+10: Title=Connect 55; Price=135
+11: Title=Connect First Responder; Price=105
+12: Title=Connect Next; Price=180
+13: Title=Connect Military; Price=105</t>
+  </si>
+  <si>
+    <t>plan_for_lines(Num, Title, Price) :-
+    plan(Title, _, lines(Ls), _),
+    member(line(Num, monthly_price(Price), _), Ls).</t>
+  </si>
+  <si>
+    <t>plan_for_lines(3, Title, Price).</t>
+  </si>
+  <si>
+    <t>Are there any special plans for veterans and if so  list them and also list if taxes and fees are included in the price.</t>
+  </si>
+  <si>
+    <t>1: Title=Connect Next Military; TaxesIncluded=yes
+2: Title=Connect Plus Military; TaxesIncluded=yes
+3: Title=Connect Military; TaxesIncluded=yes</t>
+  </si>
+  <si>
+    <t>veteran_plan(Title, TaxesIncluded) :- 
+    plan(Title, category(military_veteran), _Lines, features(Features)), 
+    member(feature(taxes_and_fees(_, included_in_monthly_price(TaxesIncluded)), _), Features).</t>
+  </si>
+  <si>
+    <t>veteran_plan(Title, TaxesIncluded).</t>
+  </si>
+  <si>
+    <t>What categories of plans are available?</t>
+  </si>
+  <si>
+    <t>Categories=[55_plus,all,first_responder,military_veteran]"</t>
+  </si>
+  <si>
+    <t>setof(Category, Title^Lines^Features^(plan(Title, category(Category), Lines, Features)), Categories).</t>
+  </si>
+  <si>
+    <t>Included=no</t>
+  </si>
+  <si>
+    <t>%% Helper predicate to check if a feature applies to a given line number
+feature_applies_for_line(applies_to_lines(all), _Line).
+feature_applies_for_line(applies_to_lines(lines(Low,High)), Line) :- Line &gt;= Low, Line =&lt; High.
+%% Predicate to check if the netflix feature is included for a given plan title and number of lines
+plan_netflix_included(PlanTitle, NumLines, Included) :-
+    plan(PlanTitle, _, lines(Lines), features(Features)),
+    %% Ensure the plan supports the requested number of lines
+    member(line(NumLines, monthly_price(_), _), Lines),
+    (   %% If there's a netflix feature that applies to the given line
+        member(feature(netflix(_, included(Inc)), Appl), Features),
+        feature_applies_for_line(Appl, NumLines)
+    -&gt;  Included = Inc
+    ;   %% Otherwise, netflix is not included
+        Included = no
+    ).</t>
+  </si>
+  <si>
+    <t>plan_netflix_included('Core', 1, Included).</t>
+  </si>
+  <si>
+    <t>I want to purchase 1 line of 'Core'. Is netflix included?</t>
+  </si>
+  <si>
+    <t>Title=Connect 55; Lines=1; Price=60</t>
+  </si>
+  <si>
+    <t>candidate_55_netflix_plan(Title, Lines, Price) :-
+    plan(Title, category("55_plus"), lines(LinesList), features(Features)),
+    member(line(Lines, monthly_price(Price), _), LinesList),
+    member(feature(netflix(_, included(yes)), _), Features).
+cheapest_55_netflix_plan(Title, Lines, Price) :-
+    setof((P, N, T), candidate_55_netflix_plan(T, N, P), Sorted),
+    Sorted = [(Price, Lines, Title)|_].</t>
+  </si>
+  <si>
+    <t>cheapest_55_netflix_plan(Title, Lines, Price).</t>
+  </si>
+  <si>
+    <t>I am over 55 and am looking for the cheapest plan where netflix is included. Give the price and the number of lines</t>
   </si>
 </sst>
 </file>
@@ -464,13 +595,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6B63DAB2-8627-834F-B841-1ECC0EE8C208}">
-  <dimension ref="A1:D5"/>
+  <dimension ref="A1:D11"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+      <selection activeCell="A11" sqref="A11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="16" x14ac:dyDescent="0.4"/>
   <cols>
     <col min="1" max="1" width="38.6640625" style="1" customWidth="1"/>
     <col min="2" max="2" width="46.1640625" style="1" customWidth="1"/>
@@ -478,7 +609,7 @@
     <col min="4" max="4" width="45.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -492,7 +623,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="102" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:4" ht="102" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A2" s="1" t="s">
         <v>3</v>
       </c>
@@ -503,7 +634,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:4" ht="140" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:4" ht="140" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A3" s="1" t="s">
         <v>6</v>
       </c>
@@ -517,7 +648,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="4" spans="1:4" ht="102" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:4" ht="96" x14ac:dyDescent="0.4">
       <c r="A4" s="1" t="s">
         <v>14</v>
       </c>
@@ -531,9 +662,99 @@
         <v>13</v>
       </c>
     </row>
-    <row r="5" spans="1:4" ht="34" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:4" ht="112" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A5" s="1" t="s">
         <v>15</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="D5" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" ht="64" x14ac:dyDescent="0.4">
+      <c r="A6" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" ht="208" x14ac:dyDescent="0.4">
+      <c r="A7" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" ht="96" x14ac:dyDescent="0.4">
+      <c r="A8" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="D8" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" ht="32" x14ac:dyDescent="0.4">
+      <c r="A9" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" ht="409.5" x14ac:dyDescent="0.4">
+      <c r="A10" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" ht="192" x14ac:dyDescent="0.4">
+      <c r="A11" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>40</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
windows attempt (not working)
</commit_message>
<xml_diff>
--- a/src/Samples/PlanSelection/PlanAssistant/scripts/TestSet.xlsx
+++ b/src/Samples/PlanSelection/PlanAssistant/scripts/TestSet.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\s\repos\RTOpenAI\src\Samples\PlanSelection\PlanAssistant\scripts\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{79407D8F-DA5C-4F7C-B367-8D9064A8C6A8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B7756898-11B4-4FAA-B42F-F211267E9474}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-20600" yWindow="610" windowWidth="20550" windowHeight="16780" xr2:uid="{92FAE82D-58B3-3F4F-8F03-CAD8585F1368}"/>
+    <workbookView xWindow="-30800" yWindow="2370" windowWidth="28290" windowHeight="15350" xr2:uid="{92FAE82D-58B3-3F4F-8F03-CAD8585F1368}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -597,8 +597,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6B63DAB2-8627-834F-B841-1ECC0EE8C208}">
   <dimension ref="A1:D11"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="A11" sqref="A11"/>
+    <sheetView tabSelected="1" topLeftCell="A10" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="16" x14ac:dyDescent="0.4"/>

</xml_diff>